<commit_message>
aggiornate info in "report-checklist"
valorizzata colonna "O" con il messaggio di errore
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#AFFIDEAXX/AFFIDEA/AffideaHCIS-RIS/V.12.0/accreditamento-checklist_V8.2.6-RIS.xlsx
+++ b/GATEWAY/A1#111#AFFIDEAXX/AFFIDEA/AffideaHCIS-RIS/V.12.0/accreditamento-checklist_V8.2.6-RIS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ombretta.bonino\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DCBA78-A79E-4E98-BA26-4021DFAE99E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1FA7A9-F1C6-4CD6-833A-E9F2DA8A7009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5400" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-645" yWindow="-16965" windowWidth="27555" windowHeight="15660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="528">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1925,6 +1925,69 @@
 Firmato digitalmente il referto è inserito nel repository per la pubblicazione.
 Attualmente AffideaHCIS-RIS non pubblica direttamente il referto verso FSE. 
 AffideaHCIS-RIS è integrato con un altro software validato che si occupa della integrazioni regionali e pubblicazioni su FSE.</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [Errore-46| codice fiscale 'nnmnnm56r28l219a' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i suoi sotto-elementi 'country', 'city' e 'streetAddressLine'.   ]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 400] [Errore vocabolario.] Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: X]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 400] [Errore vocabolario.] Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.2.7 v1.0.0, Codes: 99]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 400] [Errore di sintassi.] ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":priorityCode}'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id}' is expected."</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 400] [Errore di sintassi.] ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":text}'. One of '{\"urn:hl7-org:v3\":id, \"urn:hl7-org:v3\":code}' is expected.</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-b4| Sezione Referto: DEVE essere presente la sezione \"Referto\".],[ERRORE-b5| Sezione Referto: La sezione deve contenere l'elemento 'text'.]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-b13| Sezione Precedenti Esami Eseguiti: La section deve contenere l'elemento 'text'.]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-b7| Sezione Dicom Object Catalog: La sezione deve avere l'elemento 'entry' di tipo 'act'.]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-b22| Sezione Storia Clinica: L'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato.]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-b26| Sezione Storia Clinica: La entry/organizer deve avere un elemento subject/relatedSubject il quale deve contenere l'elemento 'code'. ]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-b53| Sotto sezione Allergie: I'elemento entry/act/entryRelationship/observation/effectiveTime deve avere valorizzato l'elemento 'low'.]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-b57| Sotto sezione Allergie: L'elemento entryRelationship/observation (Descrizione Agente) deve avere almeno un elemento 'participant' che dettaglia l'agente scatenante.]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 400] [Errore vocabolario.] Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 777.7]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 422] [Errore semantico.] [ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 400] [Errore di sintassi.] ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":languageCode}'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected.</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 400] [Errore vocabolario.] Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: ff]</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 403] [Campo token JWT non valido.] Il campo purpose_of_use non è valorizzato</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Http Status Code 403] [Campo token JWT non valido.] Il campo action_id non è corretto</t>
+  </si>
+  <si>
+    <t>Validazione FSE Gateway: [Timeout o annullamento] L'operazione è stata annullata o ha impiegato troppo tempo. The request was canceled due to the configured HttpClient.Timeout of 0,001 seconds elapsing.</t>
   </si>
 </sst>
 </file>
@@ -2407,7 +2470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2596,6 +2659,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4054,10 +4123,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F179" sqref="F179"/>
+      <pane xSplit="4" ySplit="13" topLeftCell="N14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="P64" sqref="P64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4533,7 +4602,9 @@
       <c r="N14" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O14" s="38"/>
+      <c r="O14" s="35" t="s">
+        <v>525</v>
+      </c>
       <c r="P14" s="38" t="s">
         <v>64</v>
       </c>
@@ -4851,7 +4922,9 @@
       <c r="N22" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O22" s="38"/>
+      <c r="O22" s="35" t="s">
+        <v>526</v>
+      </c>
       <c r="P22" s="38" t="s">
         <v>64</v>
       </c>
@@ -5167,7 +5240,9 @@
       <c r="N30" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O30" s="38"/>
+      <c r="O30" s="35" t="s">
+        <v>527</v>
+      </c>
       <c r="P30" s="38" t="s">
         <v>64</v>
       </c>
@@ -6050,7 +6125,9 @@
       <c r="N53" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O53" s="38"/>
+      <c r="O53" s="73" t="s">
+        <v>507</v>
+      </c>
       <c r="P53" s="38" t="s">
         <v>64</v>
       </c>
@@ -6109,7 +6186,9 @@
       <c r="N54" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O54" s="38"/>
+      <c r="O54" s="73" t="s">
+        <v>508</v>
+      </c>
       <c r="P54" s="38" t="s">
         <v>64</v>
       </c>
@@ -6168,7 +6247,9 @@
       <c r="N55" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O55" s="38"/>
+      <c r="O55" s="73" t="s">
+        <v>509</v>
+      </c>
       <c r="P55" s="38" t="s">
         <v>64</v>
       </c>
@@ -6227,7 +6308,9 @@
       <c r="N56" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O56" s="38"/>
+      <c r="O56" s="73" t="s">
+        <v>510</v>
+      </c>
       <c r="P56" s="38" t="s">
         <v>64</v>
       </c>
@@ -6286,7 +6369,9 @@
       <c r="N57" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O57" s="38"/>
+      <c r="O57" s="73" t="s">
+        <v>511</v>
+      </c>
       <c r="P57" s="38" t="s">
         <v>64</v>
       </c>
@@ -6345,7 +6430,9 @@
       <c r="N58" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O58" s="38"/>
+      <c r="O58" s="73" t="s">
+        <v>512</v>
+      </c>
       <c r="P58" s="38" t="s">
         <v>64</v>
       </c>
@@ -6404,7 +6491,9 @@
       <c r="N59" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O59" s="38"/>
+      <c r="O59" s="73" t="s">
+        <v>513</v>
+      </c>
       <c r="P59" s="38" t="s">
         <v>64</v>
       </c>
@@ -6463,7 +6552,9 @@
       <c r="N60" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O60" s="38"/>
+      <c r="O60" s="73" t="s">
+        <v>514</v>
+      </c>
       <c r="P60" s="38" t="s">
         <v>64</v>
       </c>
@@ -6522,7 +6613,9 @@
       <c r="N61" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O61" s="38"/>
+      <c r="O61" s="73" t="s">
+        <v>515</v>
+      </c>
       <c r="P61" s="38" t="s">
         <v>64</v>
       </c>
@@ -6581,7 +6674,9 @@
       <c r="N62" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O62" s="38"/>
+      <c r="O62" s="73" t="s">
+        <v>516</v>
+      </c>
       <c r="P62" s="38" t="s">
         <v>64</v>
       </c>
@@ -6640,7 +6735,9 @@
       <c r="N63" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O63" s="38"/>
+      <c r="O63" s="73" t="s">
+        <v>517</v>
+      </c>
       <c r="P63" s="38" t="s">
         <v>64</v>
       </c>
@@ -6699,7 +6796,9 @@
       <c r="N64" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O64" s="38"/>
+      <c r="O64" s="73" t="s">
+        <v>518</v>
+      </c>
       <c r="P64" s="38" t="s">
         <v>64</v>
       </c>
@@ -6758,7 +6857,9 @@
       <c r="N65" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O65" s="38"/>
+      <c r="O65" s="73" t="s">
+        <v>519</v>
+      </c>
       <c r="P65" s="38" t="s">
         <v>64</v>
       </c>
@@ -6817,7 +6918,9 @@
       <c r="N66" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O66" s="38"/>
+      <c r="O66" s="73" t="s">
+        <v>520</v>
+      </c>
       <c r="P66" s="38" t="s">
         <v>64</v>
       </c>
@@ -6876,7 +6979,9 @@
       <c r="N67" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O67" s="38"/>
+      <c r="O67" s="73" t="s">
+        <v>521</v>
+      </c>
       <c r="P67" s="38" t="s">
         <v>64</v>
       </c>
@@ -6935,7 +7040,9 @@
       <c r="N68" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O68" s="38"/>
+      <c r="O68" s="73" t="s">
+        <v>522</v>
+      </c>
       <c r="P68" s="38" t="s">
         <v>64</v>
       </c>
@@ -11064,7 +11171,9 @@
       <c r="N179" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O179" s="35"/>
+      <c r="O179" s="73" t="s">
+        <v>523</v>
+      </c>
       <c r="P179" s="38" t="s">
         <v>64</v>
       </c>
@@ -11415,7 +11524,7 @@
       <c r="L188" s="49"/>
       <c r="M188" s="49"/>
       <c r="N188" s="49"/>
-      <c r="O188" s="49"/>
+      <c r="O188" s="74"/>
       <c r="P188" s="49"/>
       <c r="Q188" s="49"/>
       <c r="R188" s="49"/>
@@ -11462,7 +11571,7 @@
       <c r="L189" s="49"/>
       <c r="M189" s="49"/>
       <c r="N189" s="49"/>
-      <c r="O189" s="49"/>
+      <c r="O189" s="74"/>
       <c r="P189" s="49"/>
       <c r="Q189" s="49"/>
       <c r="R189" s="49"/>
@@ -11550,7 +11659,9 @@
       <c r="N191" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="O191" s="38"/>
+      <c r="O191" s="73" t="s">
+        <v>524</v>
+      </c>
       <c r="P191" s="38" t="s">
         <v>64</v>
       </c>
@@ -17926,27 +18037,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -18204,32 +18294,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18248,6 +18334,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>